<commit_message>
added greener consistant grass and chests
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nyororo\Documents\ESSGAME\Town-Builder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Time sheet</t>
   </si>
@@ -39,13 +44,19 @@
     <t>Person</t>
   </si>
   <si>
-    <t>Evan</t>
+    <t>Evan F</t>
+  </si>
+  <si>
+    <t>Evan S</t>
+  </si>
+  <si>
+    <t>Made smoother green grass and made chest sprites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +195,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -195,6 +212,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -243,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,9 +296,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,6 +348,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,7 +544,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +583,7 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>42769</v>
@@ -545,11 +599,21 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11">
+        <v>42771</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>

</xml_diff>

<commit_message>
trying to do this thing again
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nyororo\Documents\ESSGAME\Town-Builder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Time sheet</t>
   </si>
@@ -52,12 +57,18 @@
   </si>
   <si>
     <t>Frost, Evan</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Made basic water, sand, and birch tree, fall and spring/summer.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -297,9 +308,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,6 +360,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,7 +556,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,12 +661,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="12"/>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
+        <v>42774</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>

</xml_diff>